<commit_message>
bugfixes; the FilterTransmission class seems to work ok!
</commit_message>
<xml_diff>
--- a/zeustools/data/hdpe.xlsx
+++ b/zeustools/data/hdpe.xlsx
@@ -1,21 +1,33 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25225"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Christopher\Dropbox\Documents\zeus2\grating_and_filter_docs\FilterData_CR\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl$\Ubuntu\home\christopher\code\zeustools\zeustools\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:40009_{C317F9D8-C17F-42CF-91C1-69F59C45E340}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{958754A0-D486-41DD-AEBD-536678E50821}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="38280" yWindow="3360" windowWidth="19440" windowHeight="15600"/>
+    <workbookView xWindow="37170" yWindow="7800" windowWidth="2400" windowHeight="585" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="wavenumber-nepers-hdpe" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
@@ -49,13 +61,13 @@
     <t>value from technical drawing</t>
   </si>
   <si>
-    <t>&lt;- from Birch &amp; Dromey 1981</t>
+    <t>HDPE data from Birch &amp; Dromey 1981</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -644,7 +656,7 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>'wavenumber-nepers-hdpe'!$D$2:$D$45</c:f>
+              <c:f>'wavenumber-nepers-hdpe'!$D$3:$D$46</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="44"/>
@@ -785,7 +797,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>'wavenumber-nepers-hdpe'!$C$2:$C$45</c:f>
+              <c:f>'wavenumber-nepers-hdpe'!$C$3:$C$46</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="44"/>
@@ -961,7 +973,7 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>'wavenumber-nepers-hdpe'!$L$4:$L$8</c:f>
+              <c:f>'wavenumber-nepers-hdpe'!$L$5:$L$9</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
@@ -985,7 +997,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>'wavenumber-nepers-hdpe'!$M$4:$M$8</c:f>
+              <c:f>'wavenumber-nepers-hdpe'!$M$5:$M$9</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
@@ -1763,13 +1775,13 @@
     <xdr:from>
       <xdr:col>5</xdr:col>
       <xdr:colOff>533400</xdr:colOff>
-      <xdr:row>21</xdr:row>
+      <xdr:row>22</xdr:row>
       <xdr:rowOff>28575</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>13</xdr:col>
       <xdr:colOff>228600</xdr:colOff>
-      <xdr:row>35</xdr:row>
+      <xdr:row>36</xdr:row>
       <xdr:rowOff>104775</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
@@ -2094,809 +2106,815 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:M46"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:M47"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
+      <selection activeCell="D1" sqref="D1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
+      <c r="D1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B2" t="s">
         <v>5</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C2" t="s">
         <v>1</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D2" t="s">
         <v>2</v>
       </c>
-      <c r="E1" t="s">
-        <v>9</v>
-      </c>
-      <c r="G1" t="s">
+      <c r="G2" t="s">
         <v>3</v>
       </c>
-      <c r="H1">
+      <c r="H2">
         <v>0.3175</v>
       </c>
-      <c r="I1" t="s">
+      <c r="I2" t="s">
         <v>4</v>
       </c>
-      <c r="J1" s="1">
+      <c r="J2" s="1">
         <f>1/8</f>
         <v>0.125</v>
       </c>
-      <c r="K1" t="s">
-        <v>6</v>
-      </c>
-      <c r="L1" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A2">
-        <v>5.4411188932875101</v>
-      </c>
-      <c r="B2">
-        <v>1.6083003436725099E-2</v>
-      </c>
-      <c r="C2">
-        <f>EXP(-B2*$H$1*2)</f>
-        <v>0.98983926543416489</v>
-      </c>
-      <c r="D2">
-        <f>10000/A2</f>
-        <v>1837.857285628623</v>
-      </c>
-      <c r="H2">
-        <f>J2*2.54</f>
-        <v>0.59943999999999997</v>
-      </c>
-      <c r="J2">
-        <v>0.23599999999999999</v>
-      </c>
       <c r="K2" t="s">
         <v>6</v>
       </c>
       <c r="L2" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A3">
-        <v>5.9349632400922196</v>
+        <v>5.4411188932875101</v>
       </c>
       <c r="B3">
-        <v>1.7756993083046901E-2</v>
+        <v>1.6083003436725099E-2</v>
       </c>
       <c r="C3">
-        <f>EXP(-B3*$H$1*2)</f>
-        <v>0.98878764172949007</v>
+        <f t="shared" ref="C3:C46" si="0">EXP(-B3*$H$2*2)</f>
+        <v>0.98983926543416489</v>
       </c>
       <c r="D3">
-        <f>10000/A3</f>
-        <v>1684.9304023397146</v>
+        <f t="shared" ref="D3:D46" si="1">10000/A3</f>
+        <v>1837.857285628623</v>
+      </c>
+      <c r="H3">
+        <f>J3*2.54</f>
+        <v>0.59943999999999997</v>
+      </c>
+      <c r="J3">
+        <v>0.23599999999999999</v>
+      </c>
+      <c r="K3" t="s">
+        <v>6</v>
+      </c>
+      <c r="L3" t="s">
+        <v>7</v>
       </c>
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A4">
-        <v>6.4285465698003197</v>
+        <v>5.9349632400922196</v>
       </c>
       <c r="B4">
-        <v>1.9007264975855899E-2</v>
+        <v>1.7756993083046901E-2</v>
       </c>
       <c r="C4">
-        <f>EXP(-B4*$H$1*2)</f>
-        <v>0.98800293236325709</v>
+        <f t="shared" si="0"/>
+        <v>0.98878764172949007</v>
       </c>
       <c r="D4">
-        <f>10000/A4</f>
-        <v>1555.5615707876275</v>
-      </c>
-      <c r="L4">
-        <v>200</v>
-      </c>
-      <c r="M4">
-        <v>0.70860000000000001</v>
+        <f t="shared" si="1"/>
+        <v>1684.9304023397146</v>
       </c>
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A5">
-        <v>6.8588332535780996</v>
+        <v>6.4285465698003197</v>
       </c>
       <c r="B5">
-        <v>1.75059816417973E-2</v>
+        <v>1.9007264975855899E-2</v>
       </c>
       <c r="C5">
-        <f>EXP(-B5*$H$1*2)</f>
-        <v>0.98894525939268507</v>
+        <f t="shared" si="0"/>
+        <v>0.98800293236325709</v>
       </c>
       <c r="D5">
-        <f>10000/A5</f>
-        <v>1457.9739192206232</v>
+        <f t="shared" si="1"/>
+        <v>1555.5615707876275</v>
       </c>
       <c r="L5">
-        <v>310</v>
+        <v>200</v>
       </c>
       <c r="M5">
-        <v>0.81459999999999999</v>
+        <v>0.70860000000000001</v>
       </c>
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A6">
-        <v>7.3943315787183996</v>
+        <v>6.8588332535780996</v>
       </c>
       <c r="B6">
-        <v>2.0131596119545701E-2</v>
+        <v>1.75059816417973E-2</v>
       </c>
       <c r="C6">
-        <f>EXP(-B6*$H$1*2)</f>
-        <v>0.98729779914174864</v>
+        <f t="shared" si="0"/>
+        <v>0.98894525939268507</v>
       </c>
       <c r="D6">
-        <f>10000/A6</f>
-        <v>1352.3872839001385</v>
+        <f t="shared" si="1"/>
+        <v>1457.9739192206232</v>
       </c>
       <c r="L6">
-        <v>353</v>
+        <v>310</v>
       </c>
       <c r="M6">
-        <v>0.84050000000000002</v>
+        <v>0.81459999999999999</v>
       </c>
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A7">
-        <v>7.9106016444077003</v>
+        <v>7.3943315787183996</v>
       </c>
       <c r="B7">
-        <v>2.4876669421847099E-2</v>
+        <v>2.0131596119545701E-2</v>
       </c>
       <c r="C7">
-        <f>EXP(-B7*$H$1*2)</f>
-        <v>0.98432742816159691</v>
+        <f t="shared" si="0"/>
+        <v>0.98729779914174864</v>
       </c>
       <c r="D7">
-        <f>10000/A7</f>
-        <v>1264.1263521428075</v>
+        <f t="shared" si="1"/>
+        <v>1352.3872839001385</v>
       </c>
       <c r="L7">
-        <v>455</v>
+        <v>353</v>
       </c>
       <c r="M7">
-        <v>0.86670000000000003</v>
+        <v>0.84050000000000002</v>
       </c>
     </row>
     <row r="8" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A8">
-        <v>8.3646843868273297</v>
+        <v>7.9106016444077003</v>
       </c>
       <c r="B8">
-        <v>2.8670987949710701E-2</v>
+        <v>2.4876669421847099E-2</v>
       </c>
       <c r="C8">
-        <f>EXP(-B8*$H$1*2)</f>
-        <v>0.9819586520710909</v>
+        <f t="shared" si="0"/>
+        <v>0.98432742816159691</v>
       </c>
       <c r="D8">
-        <f>10000/A8</f>
-        <v>1195.5023689534489</v>
+        <f t="shared" si="1"/>
+        <v>1264.1263521428075</v>
       </c>
       <c r="L8">
-        <v>621</v>
+        <v>455</v>
       </c>
       <c r="M8">
-        <v>0.88270000000000004</v>
+        <v>0.86670000000000003</v>
       </c>
     </row>
     <row r="9" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A9">
-        <v>8.8368208117631699</v>
+        <v>8.3646843868273297</v>
       </c>
       <c r="B9">
-        <v>2.84391177622134E-2</v>
+        <v>2.8670987949710701E-2</v>
       </c>
       <c r="C9">
-        <f>EXP(-B9*$H$1*2)</f>
-        <v>0.98210324392035508</v>
+        <f t="shared" si="0"/>
+        <v>0.9819586520710909</v>
       </c>
       <c r="D9">
-        <f>10000/A9</f>
-        <v>1131.6286946419077</v>
+        <f t="shared" si="1"/>
+        <v>1195.5023689534489</v>
+      </c>
+      <c r="L9">
+        <v>621</v>
+      </c>
+      <c r="M9">
+        <v>0.88270000000000004</v>
       </c>
     </row>
     <row r="10" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A10">
-        <v>9.3708182885978992</v>
+        <v>8.8368208117631699</v>
       </c>
       <c r="B10">
-        <v>2.8628355157262801E-2</v>
+        <v>2.84391177622134E-2</v>
       </c>
       <c r="C10">
-        <f>EXP(-B10*$H$1*2)</f>
-        <v>0.98198523584194775</v>
+        <f t="shared" si="0"/>
+        <v>0.98210324392035508</v>
       </c>
       <c r="D10">
-        <f>10000/A10</f>
-        <v>1067.142664815907</v>
+        <f t="shared" si="1"/>
+        <v>1131.6286946419077</v>
       </c>
     </row>
     <row r="11" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A11">
-        <v>9.8256840823073901</v>
+        <v>9.3708182885978992</v>
       </c>
       <c r="B11">
-        <v>3.3693826945664897E-2</v>
+        <v>2.8628355157262801E-2</v>
       </c>
       <c r="C11">
-        <f>EXP(-B11*$H$1*2)</f>
-        <v>0.97883168162901868</v>
+        <f t="shared" si="0"/>
+        <v>0.98198523584194775</v>
       </c>
       <c r="D11">
-        <f>10000/A11</f>
-        <v>1017.7408429003424</v>
+        <f t="shared" si="1"/>
+        <v>1067.142664815907</v>
       </c>
     </row>
     <row r="12" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A12">
-        <v>10.320441988950201</v>
+        <v>9.8256840823073901</v>
       </c>
       <c r="B12">
-        <v>3.68508287292817E-2</v>
+        <v>3.3693826945664897E-2</v>
       </c>
       <c r="C12">
-        <f>EXP(-B12*$H$1*2)</f>
-        <v>0.97687138709633181</v>
+        <f t="shared" si="0"/>
+        <v>0.97883168162901868</v>
       </c>
       <c r="D12">
-        <f>10000/A12</f>
-        <v>968.95074946467514</v>
+        <f t="shared" si="1"/>
+        <v>1017.7408429003424</v>
       </c>
     </row>
     <row r="13" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A13">
-        <v>10.81389481011</v>
+        <v>10.320441988950201</v>
       </c>
       <c r="B13">
-        <v>3.7889241745334298E-2</v>
+        <v>3.68508287292817E-2</v>
       </c>
       <c r="C13">
-        <f>EXP(-B13*$H$1*2)</f>
-        <v>0.97622745798386135</v>
+        <f t="shared" si="0"/>
+        <v>0.97687138709633181</v>
       </c>
       <c r="D13">
-        <f>10000/A13</f>
-        <v>924.73620056401114</v>
+        <f t="shared" si="1"/>
+        <v>968.95074946467514</v>
       </c>
     </row>
     <row r="14" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A14">
-        <v>11.287336320528899</v>
+        <v>10.81389481011</v>
       </c>
       <c r="B14">
-        <v>3.9775960325401302E-2</v>
+        <v>3.7889241745334298E-2</v>
       </c>
       <c r="C14">
-        <f>EXP(-B14*$H$1*2)</f>
-        <v>0.9750585731075373</v>
+        <f t="shared" si="0"/>
+        <v>0.97622745798386135</v>
       </c>
       <c r="D14">
-        <f>10000/A14</f>
-        <v>885.94861675313507</v>
+        <f t="shared" si="1"/>
+        <v>924.73620056401114</v>
       </c>
     </row>
     <row r="15" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A15">
-        <v>11.7814416844303</v>
+        <v>11.287336320528899</v>
       </c>
       <c r="B15">
-        <v>4.1873667725236E-2</v>
+        <v>3.9775960325401302E-2</v>
       </c>
       <c r="C15">
-        <f>EXP(-B15*$H$1*2)</f>
-        <v>0.97376061665124869</v>
+        <f t="shared" si="0"/>
+        <v>0.9750585731075373</v>
       </c>
       <c r="D15">
-        <f>10000/A15</f>
-        <v>848.79255594121776</v>
+        <f t="shared" si="1"/>
+        <v>885.94861675313507</v>
       </c>
     </row>
     <row r="16" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A16">
-        <v>12.2554052290425</v>
+        <v>11.7814416844303</v>
       </c>
       <c r="B16">
-        <v>4.4607821812328703E-2</v>
+        <v>4.1873667725236E-2</v>
       </c>
       <c r="C16">
-        <f>EXP(-B16*$H$1*2)</f>
-        <v>0.97207145208219081</v>
+        <f t="shared" si="0"/>
+        <v>0.97376061665124869</v>
       </c>
       <c r="D16">
-        <f>10000/A16</f>
-        <v>815.96649095717316</v>
+        <f t="shared" si="1"/>
+        <v>848.79255594121776</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17">
-        <v>12.748336016009</v>
+        <v>12.2554052290425</v>
       </c>
       <c r="B17">
-        <v>4.4798799321355498E-2</v>
+        <v>4.4607821812328703E-2</v>
       </c>
       <c r="C17">
-        <f>EXP(-B17*$H$1*2)</f>
-        <v>0.97195357542666172</v>
+        <f t="shared" si="0"/>
+        <v>0.97207145208219081</v>
       </c>
       <c r="D17">
-        <f>10000/A17</f>
-        <v>784.41609849648478</v>
+        <f t="shared" si="1"/>
+        <v>815.96649095717316</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18">
-        <v>13.264279810327499</v>
+        <v>12.748336016009</v>
       </c>
       <c r="B18">
-        <v>4.9014225431765701E-2</v>
+        <v>4.4798799321355498E-2</v>
       </c>
       <c r="C18">
-        <f>EXP(-B18*$H$1*2)</f>
-        <v>0.96935533342465818</v>
+        <f t="shared" si="0"/>
+        <v>0.97195357542666172</v>
       </c>
       <c r="D18">
-        <f>10000/A18</f>
-        <v>753.90448203709127</v>
+        <f t="shared" si="1"/>
+        <v>784.41609849648478</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19">
-        <v>13.717840518553899</v>
+        <v>13.264279810327499</v>
       </c>
       <c r="B19">
-        <v>5.1961108452603599E-2</v>
+        <v>4.9014225431765701E-2</v>
       </c>
       <c r="C19">
-        <f>EXP(-B19*$H$1*2)</f>
-        <v>0.96754310328906923</v>
+        <f t="shared" si="0"/>
+        <v>0.96935533342465818</v>
       </c>
       <c r="D19">
-        <f>10000/A19</f>
-        <v>728.97771237933705</v>
+        <f t="shared" si="1"/>
+        <v>753.90448203709127</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20">
-        <v>14.2118153739069</v>
+        <v>13.717840518553899</v>
       </c>
       <c r="B20">
-        <v>5.3846956975681898E-2</v>
+        <v>5.1961108452603599E-2</v>
       </c>
       <c r="C20">
-        <f>EXP(-B20*$H$1*2)</f>
-        <v>0.96638515052961627</v>
+        <f t="shared" si="0"/>
+        <v>0.96754310328906923</v>
       </c>
       <c r="D20">
-        <f>10000/A20</f>
-        <v>703.63987547714316</v>
+        <f t="shared" si="1"/>
+        <v>728.97771237933705</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21">
-        <v>14.666028624874899</v>
+        <v>14.2118153739069</v>
       </c>
       <c r="B21">
-        <v>5.7853134380301902E-2</v>
+        <v>5.3846956975681898E-2</v>
       </c>
       <c r="C21">
-        <f>EXP(-B21*$H$1*2)</f>
-        <v>0.96392986580602735</v>
+        <f t="shared" si="0"/>
+        <v>0.96638515052961627</v>
       </c>
       <c r="D21">
-        <f>10000/A21</f>
-        <v>681.84784414228568</v>
+        <f t="shared" si="1"/>
+        <v>703.63987547714316</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22">
-        <v>15.220820463740299</v>
+        <v>14.666028624874899</v>
       </c>
       <c r="B22">
-        <v>5.8465219471875399E-2</v>
+        <v>5.7853134380301902E-2</v>
       </c>
       <c r="C22">
-        <f>EXP(-B22*$H$1*2)</f>
-        <v>0.96355528409721891</v>
+        <f t="shared" si="0"/>
+        <v>0.96392986580602735</v>
       </c>
       <c r="D22">
-        <f>10000/A22</f>
-        <v>656.99480680574584</v>
+        <f t="shared" si="1"/>
+        <v>681.84784414228568</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23">
-        <v>15.6324009222604</v>
+        <v>15.220820463740299</v>
       </c>
       <c r="B23">
-        <v>5.99308304693957E-2</v>
+        <v>5.8465219471875399E-2</v>
       </c>
       <c r="C23">
-        <f>EXP(-B23*$H$1*2)</f>
-        <v>0.96265895601620377</v>
+        <f t="shared" si="0"/>
+        <v>0.96355528409721891</v>
       </c>
       <c r="D23">
-        <f>10000/A23</f>
-        <v>639.69700174207333</v>
+        <f t="shared" si="1"/>
+        <v>656.99480680574584</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24">
-        <v>16.1665289076434</v>
+        <v>15.6324009222604</v>
       </c>
       <c r="B24">
-        <v>6.0331926741201497E-2</v>
+        <v>5.99308304693957E-2</v>
       </c>
       <c r="C24">
-        <f>EXP(-B24*$H$1*2)</f>
-        <v>0.9624138017243471</v>
+        <f t="shared" si="0"/>
+        <v>0.96265895601620377</v>
       </c>
       <c r="D24">
-        <f>10000/A24</f>
-        <v>618.56197190678847</v>
+        <f t="shared" si="1"/>
+        <v>639.69700174207333</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A25">
-        <v>16.660503762996399</v>
+        <v>16.1665289076434</v>
       </c>
       <c r="B25">
-        <v>6.2217775264279802E-2</v>
+        <v>6.0331926741201497E-2</v>
       </c>
       <c r="C25">
-        <f>EXP(-B25*$H$1*2)</f>
-        <v>0.96126198769802218</v>
+        <f t="shared" si="0"/>
+        <v>0.9624138017243471</v>
       </c>
       <c r="D25">
-        <f>10000/A25</f>
-        <v>600.22194660226137</v>
+        <f t="shared" si="1"/>
+        <v>618.56197190678847</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A26">
-        <v>17.134858833253499</v>
+        <v>16.660503762996399</v>
       </c>
       <c r="B26">
-        <v>6.5587505981641703E-2</v>
+        <v>6.2217775264279802E-2</v>
       </c>
       <c r="C26">
-        <f>EXP(-B26*$H$1*2)</f>
-        <v>0.95920729855226128</v>
+        <f t="shared" si="0"/>
+        <v>0.96126198769802218</v>
       </c>
       <c r="D26">
-        <f>10000/A26</f>
-        <v>583.60562507775501</v>
+        <f t="shared" si="1"/>
+        <v>600.22194660226137</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A27">
-        <v>18.779308546469899</v>
+        <v>17.134858833253499</v>
       </c>
       <c r="B27">
-        <v>8.5323453356222601E-2</v>
+        <v>6.5587505981641703E-2</v>
       </c>
       <c r="C27">
-        <f>EXP(-B27*$H$1*2)</f>
-        <v>0.94726121190891122</v>
+        <f t="shared" si="0"/>
+        <v>0.95920729855226128</v>
       </c>
       <c r="D27">
-        <f>10000/A27</f>
-        <v>532.50096909876811</v>
+        <f t="shared" si="1"/>
+        <v>583.60562507775501</v>
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A28">
-        <v>20.260435906908</v>
+        <v>18.779308546469899</v>
       </c>
       <c r="B28">
-        <v>9.6731784697625195E-2</v>
+        <v>8.5323453356222601E-2</v>
       </c>
       <c r="C28">
-        <f>EXP(-B28*$H$1*2)</f>
-        <v>0.94042377270332422</v>
+        <f t="shared" si="0"/>
+        <v>0.94726121190891122</v>
       </c>
       <c r="D28">
-        <f>10000/A28</f>
-        <v>493.57279606162859</v>
+        <f t="shared" si="1"/>
+        <v>532.50096909876811</v>
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A29">
-        <v>22.385319107325198</v>
+        <v>20.260435906908</v>
       </c>
       <c r="B29">
-        <v>0.107596862165627</v>
+        <v>9.6731784697625195E-2</v>
       </c>
       <c r="C29">
-        <f>EXP(-B29*$H$1*2)</f>
-        <v>0.93395781523444621</v>
+        <f t="shared" si="0"/>
+        <v>0.94042377270332422</v>
       </c>
       <c r="D29">
-        <f>10000/A29</f>
-        <v>446.72135125952605</v>
+        <f t="shared" si="1"/>
+        <v>493.57279606162859</v>
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A30">
-        <v>24.768193572220099</v>
+        <v>22.385319107325198</v>
       </c>
       <c r="B30">
-        <v>0.13090245333449099</v>
+        <v>0.107596862165627</v>
       </c>
       <c r="C30">
-        <f>EXP(-B30*$H$1*2)</f>
-        <v>0.92023789773894971</v>
+        <f t="shared" si="0"/>
+        <v>0.93395781523444621</v>
       </c>
       <c r="D30">
-        <f>10000/A30</f>
-        <v>403.74361460158957</v>
+        <f t="shared" si="1"/>
+        <v>446.72135125952605</v>
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A31">
-        <v>27.151556965601099</v>
+        <v>24.768193572220099</v>
       </c>
       <c r="B31">
-        <v>0.16686585975358001</v>
+        <v>0.13090245333449099</v>
       </c>
       <c r="C31">
-        <f>EXP(-B31*$H$1*2)</f>
-        <v>0.89946078683566144</v>
+        <f t="shared" si="0"/>
+        <v>0.92023789773894971</v>
       </c>
       <c r="D31">
-        <f>10000/A31</f>
-        <v>368.30300423173588</v>
+        <f t="shared" si="1"/>
+        <v>403.74361460158957</v>
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A32">
-        <v>28.064672999858001</v>
+        <v>27.151556965601099</v>
       </c>
       <c r="B32">
-        <v>0.174693244443341</v>
+        <v>0.16686585975358001</v>
       </c>
       <c r="C32">
-        <f>EXP(-B32*$H$1*2)</f>
-        <v>0.89500120868557154</v>
+        <f t="shared" si="0"/>
+        <v>0.89946078683566144</v>
       </c>
       <c r="D32">
-        <f>10000/A32</f>
-        <v>356.31984737718471</v>
+        <f t="shared" si="1"/>
+        <v>368.30300423173588</v>
       </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A33">
-        <v>28.924811623754</v>
+        <v>28.064672999858001</v>
       </c>
       <c r="B33">
-        <v>0.186540190206229</v>
+        <v>0.174693244443341</v>
       </c>
       <c r="C33">
-        <f>EXP(-B33*$H$1*2)</f>
-        <v>0.88829354601364108</v>
+        <f t="shared" si="0"/>
+        <v>0.89500120868557154</v>
       </c>
       <c r="D33">
-        <f>10000/A33</f>
-        <v>345.72394558959456</v>
+        <f t="shared" si="1"/>
+        <v>356.31984737718471</v>
       </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A34">
-        <v>29.784743405732499</v>
+        <v>28.924811623754</v>
       </c>
       <c r="B34">
-        <v>0.19303222855149499</v>
+        <v>0.186540190206229</v>
       </c>
       <c r="C34">
-        <f>EXP(-B34*$H$1*2)</f>
-        <v>0.8846391430163093</v>
+        <f t="shared" si="0"/>
+        <v>0.88829354601364108</v>
       </c>
       <c r="D34">
-        <f>10000/A34</f>
-        <v>335.74235855513052</v>
+        <f t="shared" si="1"/>
+        <v>345.72394558959456</v>
       </c>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A35">
-        <v>30.6448730365017</v>
+        <v>29.784743405732499</v>
       </c>
       <c r="B35">
-        <v>0.20464635225274799</v>
+        <v>0.19303222855149499</v>
       </c>
       <c r="C35">
-        <f>EXP(-B35*$H$1*2)</f>
-        <v>0.87813895595792524</v>
+        <f t="shared" si="0"/>
+        <v>0.8846391430163093</v>
       </c>
       <c r="D35">
-        <f>10000/A35</f>
-        <v>326.31885888673145</v>
+        <f t="shared" si="1"/>
+        <v>335.74235855513052</v>
       </c>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A36">
-        <v>31.504957701636599</v>
+        <v>30.6448730365017</v>
       </c>
       <c r="B36">
-        <v>0.21509636564582099</v>
+        <v>0.20464635225274799</v>
       </c>
       <c r="C36">
-        <f>EXP(-B36*$H$1*2)</f>
-        <v>0.87233112889308773</v>
+        <f t="shared" si="0"/>
+        <v>0.87813895595792524</v>
       </c>
       <c r="D36">
-        <f>10000/A36</f>
-        <v>317.41036108359947</v>
+        <f t="shared" si="1"/>
+        <v>326.31885888673145</v>
       </c>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A37">
-        <v>32.365042366771497</v>
+        <v>31.504957701636599</v>
       </c>
       <c r="B37">
-        <v>0.22554637903889399</v>
+        <v>0.21509636564582099</v>
       </c>
       <c r="C37">
-        <f>EXP(-B37*$H$1*2)</f>
-        <v>0.86656171357958656</v>
+        <f t="shared" si="0"/>
+        <v>0.87233112889308773</v>
       </c>
       <c r="D37">
-        <f>10000/A37</f>
-        <v>308.97534094584682</v>
+        <f t="shared" si="1"/>
+        <v>317.41036108359947</v>
       </c>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A38">
-        <v>33.225234949428497</v>
+        <v>32.365042366771497</v>
       </c>
       <c r="B38">
-        <v>0.23879025717159599</v>
+        <v>0.22554637903889399</v>
       </c>
       <c r="C38">
-        <f>EXP(-B38*$H$1*2)</f>
-        <v>0.85930460702813538</v>
+        <f t="shared" si="0"/>
+        <v>0.86656171357958656</v>
       </c>
       <c r="D38">
-        <f>10000/A38</f>
-        <v>300.97605074037284</v>
+        <f t="shared" si="1"/>
+        <v>308.97534094584682</v>
       </c>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A39">
-        <v>34.085292635182903</v>
+        <v>33.225234949428497</v>
       </c>
       <c r="B39">
-        <v>0.248541804379763</v>
+        <v>0.23879025717159599</v>
       </c>
       <c r="C39">
-        <f>EXP(-B39*$H$1*2)</f>
-        <v>0.85400003365820532</v>
+        <f t="shared" si="0"/>
+        <v>0.85930460702813538</v>
       </c>
       <c r="D39">
-        <f>10000/A39</f>
-        <v>293.38166777767316</v>
+        <f t="shared" si="1"/>
+        <v>300.97605074037284</v>
       </c>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A40">
-        <v>34.9451884446541</v>
+        <v>34.085292635182903</v>
       </c>
       <c r="B40">
-        <v>0.25410255447848601</v>
+        <v>0.248541804379763</v>
       </c>
       <c r="C40">
-        <f>EXP(-B40*$H$1*2)</f>
-        <v>0.85098981215698355</v>
+        <f t="shared" si="0"/>
+        <v>0.85400003365820532</v>
       </c>
       <c r="D40">
-        <f>10000/A40</f>
-        <v>286.16242879439375</v>
+        <f t="shared" si="1"/>
+        <v>293.38166777767316</v>
       </c>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A41">
-        <v>35.805057274744698</v>
+        <v>34.9451884446541</v>
       </c>
       <c r="B41">
-        <v>0.258964838392302</v>
+        <v>0.25410255447848601</v>
       </c>
       <c r="C41">
-        <f>EXP(-B41*$H$1*2)</f>
-        <v>0.84836639037710848</v>
+        <f t="shared" si="0"/>
+        <v>0.85098981215698355</v>
       </c>
       <c r="D41">
-        <f>10000/A41</f>
-        <v>279.29015511039432</v>
+        <f t="shared" si="1"/>
+        <v>286.16242879439375</v>
       </c>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A42">
-        <v>36.665870383154001</v>
+        <v>35.805057274744698</v>
       </c>
       <c r="B42">
-        <v>0.28827343877786799</v>
+        <v>0.258964838392302</v>
       </c>
       <c r="C42">
-        <f>EXP(-B42*$H$1*2)</f>
-        <v>0.83272349256072653</v>
+        <f t="shared" si="0"/>
+        <v>0.84836639037710848</v>
       </c>
       <c r="D42">
-        <f>10000/A42</f>
-        <v>272.73319562582816</v>
+        <f t="shared" si="1"/>
+        <v>279.29015511039432</v>
       </c>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A43">
-        <v>37.526683491563297</v>
+        <v>36.665870383154001</v>
       </c>
       <c r="B43">
-        <v>0.31758203916343403</v>
+        <v>0.28827343877786799</v>
       </c>
       <c r="C43">
-        <f>EXP(-B43*$H$1*2)</f>
-        <v>0.81736903173910214</v>
+        <f t="shared" si="0"/>
+        <v>0.83272349256072653</v>
       </c>
       <c r="D43">
-        <f>10000/A43</f>
-        <v>266.47705231527289</v>
+        <f t="shared" si="1"/>
+        <v>272.73319562582816</v>
       </c>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A44">
-        <v>38.387604517494701</v>
+        <v>37.526683491563297</v>
       </c>
       <c r="B44">
-        <v>0.34968450428862502</v>
+        <v>0.31758203916343403</v>
       </c>
       <c r="C44">
-        <f>EXP(-B44*$H$1*2)</f>
-        <v>0.80087559168640787</v>
+        <f t="shared" si="0"/>
+        <v>0.81736903173910214</v>
       </c>
       <c r="D44">
-        <f>10000/A44</f>
-        <v>260.50075605636232</v>
+        <f t="shared" si="1"/>
+        <v>266.47705231527289</v>
       </c>
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A45">
+        <v>38.387604517494701</v>
+      </c>
+      <c r="B45">
+        <v>0.34968450428862502</v>
+      </c>
+      <c r="C45">
+        <f t="shared" si="0"/>
+        <v>0.80087559168640787</v>
+      </c>
+      <c r="D45">
+        <f t="shared" si="1"/>
+        <v>260.50075605636232</v>
+      </c>
+    </row>
+    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A46">
         <v>38.935465804849301</v>
       </c>
-      <c r="B45">
+      <c r="B46">
         <v>0.37017684265783202</v>
       </c>
-      <c r="C45">
-        <f>EXP(-B45*$H$1*2)</f>
+      <c r="C46">
+        <f t="shared" si="0"/>
         <v>0.79052160248225001</v>
       </c>
-      <c r="D45">
-        <f>10000/A45</f>
+      <c r="D46">
+        <f t="shared" si="1"/>
         <v>256.83524758947482</v>
       </c>
     </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="C46">
+    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A47">
+        <f>10000/D47</f>
+        <v>52.631578947368418</v>
+      </c>
+      <c r="C47">
         <v>0.71</v>
       </c>
-      <c r="D46">
-        <v>200</v>
+      <c r="D47">
+        <v>190</v>
       </c>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:D50">
-    <sortCondition ref="A2:A50"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A3:D51">
+    <sortCondition ref="A3:A51"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>

</xml_diff>

<commit_message>
The ZeusOpticsChain object is now available for all your throughput-calculating needs
</commit_message>
<xml_diff>
--- a/zeustools/data/hdpe.xlsx
+++ b/zeustools/data/hdpe.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25225"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25330"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl$\Ubuntu\home\christopher\code\zeustools\zeustools\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{958754A0-D486-41DD-AEBD-536678E50821}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2FFF77FF-C6F7-4D76-9C94-004F106D7BE9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="37170" yWindow="7800" windowWidth="2400" windowHeight="585" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="38280" yWindow="3360" windowWidth="19440" windowHeight="15600" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="wavenumber-nepers-hdpe" sheetId="1" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="11">
   <si>
     <t>wavenumber</t>
   </si>
@@ -62,6 +62,9 @@
   </si>
   <si>
     <t>HDPE data from Birch &amp; Dromey 1981</t>
+  </si>
+  <si>
+    <t>note that these two are basically guesses and have no basis in reality</t>
   </si>
 </sst>
 </file>
@@ -2107,10 +2110,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:M47"/>
+  <dimension ref="A1:M48"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D1" sqref="D1"/>
+    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
+      <selection activeCell="E47" sqref="E47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2676,7 +2679,7 @@
         <v>368.30300423173588</v>
       </c>
     </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A33">
         <v>28.064672999858001</v>
       </c>
@@ -2692,7 +2695,7 @@
         <v>356.31984737718471</v>
       </c>
     </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A34">
         <v>28.924811623754</v>
       </c>
@@ -2708,7 +2711,7 @@
         <v>345.72394558959456</v>
       </c>
     </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A35">
         <v>29.784743405732499</v>
       </c>
@@ -2724,7 +2727,7 @@
         <v>335.74235855513052</v>
       </c>
     </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A36">
         <v>30.6448730365017</v>
       </c>
@@ -2740,7 +2743,7 @@
         <v>326.31885888673145</v>
       </c>
     </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A37">
         <v>31.504957701636599</v>
       </c>
@@ -2756,7 +2759,7 @@
         <v>317.41036108359947</v>
       </c>
     </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A38">
         <v>32.365042366771497</v>
       </c>
@@ -2772,7 +2775,7 @@
         <v>308.97534094584682</v>
       </c>
     </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A39">
         <v>33.225234949428497</v>
       </c>
@@ -2788,7 +2791,7 @@
         <v>300.97605074037284</v>
       </c>
     </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A40">
         <v>34.085292635182903</v>
       </c>
@@ -2804,7 +2807,7 @@
         <v>293.38166777767316</v>
       </c>
     </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A41">
         <v>34.9451884446541</v>
       </c>
@@ -2820,7 +2823,7 @@
         <v>286.16242879439375</v>
       </c>
     </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A42">
         <v>35.805057274744698</v>
       </c>
@@ -2836,7 +2839,7 @@
         <v>279.29015511039432</v>
       </c>
     </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A43">
         <v>36.665870383154001</v>
       </c>
@@ -2852,7 +2855,7 @@
         <v>272.73319562582816</v>
       </c>
     </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A44">
         <v>37.526683491563297</v>
       </c>
@@ -2868,7 +2871,7 @@
         <v>266.47705231527289</v>
       </c>
     </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A45">
         <v>38.387604517494701</v>
       </c>
@@ -2884,7 +2887,7 @@
         <v>260.50075605636232</v>
       </c>
     </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A46">
         <v>38.935465804849301</v>
       </c>
@@ -2900,7 +2903,7 @@
         <v>256.83524758947482</v>
       </c>
     </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A47">
         <f>10000/D47</f>
         <v>52.631578947368418</v>
@@ -2910,6 +2913,21 @@
       </c>
       <c r="D47">
         <v>190</v>
+      </c>
+      <c r="E47" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="48" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A48">
+        <f>10000/D48</f>
+        <v>55.555555555555557</v>
+      </c>
+      <c r="C48">
+        <v>0.6</v>
+      </c>
+      <c r="D48">
+        <v>180</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
fixed nepers conversion and other mistakes
</commit_message>
<xml_diff>
--- a/zeustools/data/hdpe.xlsx
+++ b/zeustools/data/hdpe.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl$\Ubuntu\home\christopher\code\zeustools\zeustools\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2FFF77FF-C6F7-4D76-9C94-004F106D7BE9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="14_{C4F01B96-6115-4619-9128-799C8FDA582D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="38280" yWindow="3360" windowWidth="19440" windowHeight="15600" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="wavenumber-nepers-hdpe" sheetId="1" r:id="rId1"/>
@@ -625,7 +625,17 @@
   <c:chart>
     <c:autoTitleDeleted val="0"/>
     <c:plotArea>
-      <c:layout/>
+      <c:layout>
+        <c:manualLayout>
+          <c:layoutTarget val="inner"/>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="2.8771595432489756E-2"/>
+          <c:y val="8.1733923884514444E-3"/>
+          <c:w val="0.95438215610502564"/>
+          <c:h val="0.9491097206599175"/>
+        </c:manualLayout>
+      </c:layout>
       <c:scatterChart>
         <c:scatterStyle val="lineMarker"/>
         <c:varyColors val="0"/>
@@ -805,136 +815,136 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="44"/>
                 <c:pt idx="0">
-                  <c:v>0.98983926543416489</c:v>
+                  <c:v>0.99490666166940744</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.98878764172949007</c:v>
+                  <c:v>0.99437801752124932</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.98800293236325709</c:v>
+                  <c:v>0.99398336624073202</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.98894525939268507</c:v>
+                  <c:v>0.99445726876155172</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.98729779914174864</c:v>
+                  <c:v>0.99362860221601346</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.98432742816159691</c:v>
+                  <c:v>0.99213276740645795</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0.9819586520710909</c:v>
+                  <c:v>0.99093826854708311</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0.98210324392035508</c:v>
+                  <c:v>0.99101122290333077</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>0.98198523584194775</c:v>
+                  <c:v>0.99095168189067007</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>0.97883168162901868</c:v>
+                  <c:v>0.98935922779798169</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>0.97687138709633181</c:v>
+                  <c:v>0.98836804232853048</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>0.97622745798386135</c:v>
+                  <c:v>0.98804223491906529</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>0.9750585731075373</c:v>
+                  <c:v>0.9874505421070654</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>0.97376061665124869</c:v>
+                  <c:v>0.98679309718463715</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>0.97207145208219081</c:v>
+                  <c:v>0.98593683980374258</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>0.97195357542666172</c:v>
+                  <c:v>0.98587705898182953</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>0.96935533342465818</c:v>
+                  <c:v>0.98455844591606556</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>0.96754310328906923</c:v>
+                  <c:v>0.98363768903446824</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>0.96638515052961627</c:v>
+                  <c:v>0.98304890546178636</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>0.96392986580602735</c:v>
+                  <c:v>0.98179930016578609</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>0.96355528409721891</c:v>
+                  <c:v>0.98160851875746213</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>0.96265895601620377</c:v>
+                  <c:v>0.98115185166018193</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>0.9624138017243471</c:v>
+                  <c:v>0.98102691182472013</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>0.96126198769802218</c:v>
+                  <c:v>0.9804396910050216</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>0.95920729855226128</c:v>
+                  <c:v>0.97939128980824686</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>0.94726121190891122</c:v>
+                  <c:v>0.97327345176415414</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>0.94042377270332422</c:v>
+                  <c:v>0.96975449094259125</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>0.93395781523444621</c:v>
+                  <c:v>0.96641492912436233</c:v>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>0.92023789773894971</c:v>
+                  <c:v>0.95929030941574189</c:v>
                 </c:pt>
                 <c:pt idx="29">
-                  <c:v>0.89946078683566144</c:v>
+                  <c:v>0.94839906518071881</c:v>
                 </c:pt>
                 <c:pt idx="30">
-                  <c:v>0.89500120868557154</c:v>
+                  <c:v>0.94604503523118366</c:v>
                 </c:pt>
                 <c:pt idx="31">
-                  <c:v>0.88829354601364108</c:v>
+                  <c:v>0.94249326046059401</c:v>
                 </c:pt>
                 <c:pt idx="32">
-                  <c:v>0.8846391430163093</c:v>
+                  <c:v>0.94055257323358021</c:v>
                 </c:pt>
                 <c:pt idx="33">
-                  <c:v>0.87813895595792524</c:v>
+                  <c:v>0.93709068715782529</c:v>
                 </c:pt>
                 <c:pt idx="34">
-                  <c:v>0.87233112889308773</c:v>
+                  <c:v>0.93398668560803788</c:v>
                 </c:pt>
                 <c:pt idx="35">
-                  <c:v>0.86656171357958656</c:v>
+                  <c:v>0.9308929656945456</c:v>
                 </c:pt>
                 <c:pt idx="36">
-                  <c:v>0.85930460702813538</c:v>
+                  <c:v>0.9269868429638769</c:v>
                 </c:pt>
                 <c:pt idx="37">
-                  <c:v>0.85400003365820532</c:v>
+                  <c:v>0.9241212223827594</c:v>
                 </c:pt>
                 <c:pt idx="38">
-                  <c:v>0.85098981215698355</c:v>
+                  <c:v>0.92249109055696765</c:v>
                 </c:pt>
                 <c:pt idx="39">
-                  <c:v>0.84836639037710848</c:v>
+                  <c:v>0.92106807043622374</c:v>
                 </c:pt>
                 <c:pt idx="40">
-                  <c:v>0.83272349256072653</c:v>
+                  <c:v>0.91253684449490946</c:v>
                 </c:pt>
                 <c:pt idx="41">
-                  <c:v>0.81736903173910214</c:v>
+                  <c:v>0.90408463748650336</c:v>
                 </c:pt>
                 <c:pt idx="42">
-                  <c:v>0.80087559168640787</c:v>
+                  <c:v>0.8949165277758635</c:v>
                 </c:pt>
                 <c:pt idx="43">
-                  <c:v>0.79052160248225001</c:v>
+                  <c:v>0.88911281763466332</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1026,6 +1036,86 @@
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{0000002E-EA55-4C3F-BC97-E5C0C8112D14}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:spPr>
+            <a:ln w="25400" cap="rnd">
+              <a:noFill/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent3"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent3"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>'wavenumber-nepers-hdpe'!$L$5:$L$9</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>200</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>310</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>353</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>455</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>621</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>'wavenumber-nepers-hdpe'!$N$5:$N$9</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>0.87</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.93</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.95</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.97</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.98</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-C870-4054-B4E4-F863FBE58ED8}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -1776,16 +1866,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>5</xdr:col>
-      <xdr:colOff>533400</xdr:colOff>
-      <xdr:row>22</xdr:row>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>238124</xdr:colOff>
+      <xdr:row>10</xdr:row>
       <xdr:rowOff>28575</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>13</xdr:col>
-      <xdr:colOff>228600</xdr:colOff>
-      <xdr:row>36</xdr:row>
-      <xdr:rowOff>104775</xdr:rowOff>
+      <xdr:col>27</xdr:col>
+      <xdr:colOff>342899</xdr:colOff>
+      <xdr:row>54</xdr:row>
+      <xdr:rowOff>180975</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -2110,20 +2200,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:M48"/>
+  <dimension ref="A1:N48"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
-      <selection activeCell="E47" sqref="E47"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C47" sqref="C47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
       <c r="D1" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -2156,7 +2246,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>5.4411188932875101</v>
       </c>
@@ -2164,11 +2254,11 @@
         <v>1.6083003436725099E-2</v>
       </c>
       <c r="C3">
-        <f t="shared" ref="C3:C46" si="0">EXP(-B3*$H$2*2)</f>
-        <v>0.98983926543416489</v>
+        <f>EXP(-B3*$H$2)</f>
+        <v>0.99490666166940744</v>
       </c>
       <c r="D3">
-        <f t="shared" ref="D3:D46" si="1">10000/A3</f>
+        <f t="shared" ref="D3:D46" si="0">10000/A3</f>
         <v>1837.857285628623</v>
       </c>
       <c r="H3">
@@ -2185,7 +2275,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>5.9349632400922196</v>
       </c>
@@ -2193,15 +2283,15 @@
         <v>1.7756993083046901E-2</v>
       </c>
       <c r="C4">
-        <f t="shared" si="0"/>
-        <v>0.98878764172949007</v>
+        <f t="shared" ref="C4:C46" si="1">EXP(-B4*$H$2)</f>
+        <v>0.99437801752124932</v>
       </c>
       <c r="D4">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>1684.9304023397146</v>
       </c>
     </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>6.4285465698003197</v>
       </c>
@@ -2209,11 +2299,11 @@
         <v>1.9007264975855899E-2</v>
       </c>
       <c r="C5">
-        <f t="shared" si="0"/>
-        <v>0.98800293236325709</v>
+        <f t="shared" si="1"/>
+        <v>0.99398336624073202</v>
       </c>
       <c r="D5">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>1555.5615707876275</v>
       </c>
       <c r="L5">
@@ -2222,8 +2312,11 @@
       <c r="M5">
         <v>0.70860000000000001</v>
       </c>
-    </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N5">
+        <v>0.87</v>
+      </c>
+    </row>
+    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>6.8588332535780996</v>
       </c>
@@ -2231,11 +2324,11 @@
         <v>1.75059816417973E-2</v>
       </c>
       <c r="C6">
-        <f t="shared" si="0"/>
-        <v>0.98894525939268507</v>
+        <f t="shared" si="1"/>
+        <v>0.99445726876155172</v>
       </c>
       <c r="D6">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>1457.9739192206232</v>
       </c>
       <c r="L6">
@@ -2244,8 +2337,11 @@
       <c r="M6">
         <v>0.81459999999999999</v>
       </c>
-    </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N6">
+        <v>0.93</v>
+      </c>
+    </row>
+    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>7.3943315787183996</v>
       </c>
@@ -2253,11 +2349,11 @@
         <v>2.0131596119545701E-2</v>
       </c>
       <c r="C7">
-        <f t="shared" si="0"/>
-        <v>0.98729779914174864</v>
+        <f>EXP(-B7*$H$2)</f>
+        <v>0.99362860221601346</v>
       </c>
       <c r="D7">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>1352.3872839001385</v>
       </c>
       <c r="L7">
@@ -2266,8 +2362,11 @@
       <c r="M7">
         <v>0.84050000000000002</v>
       </c>
-    </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N7">
+        <v>0.95</v>
+      </c>
+    </row>
+    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>7.9106016444077003</v>
       </c>
@@ -2275,11 +2374,11 @@
         <v>2.4876669421847099E-2</v>
       </c>
       <c r="C8">
-        <f t="shared" si="0"/>
-        <v>0.98432742816159691</v>
+        <f t="shared" si="1"/>
+        <v>0.99213276740645795</v>
       </c>
       <c r="D8">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>1264.1263521428075</v>
       </c>
       <c r="L8">
@@ -2288,8 +2387,11 @@
       <c r="M8">
         <v>0.86670000000000003</v>
       </c>
-    </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N8">
+        <v>0.97</v>
+      </c>
+    </row>
+    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>8.3646843868273297</v>
       </c>
@@ -2297,11 +2399,11 @@
         <v>2.8670987949710701E-2</v>
       </c>
       <c r="C9">
-        <f t="shared" si="0"/>
-        <v>0.9819586520710909</v>
+        <f t="shared" si="1"/>
+        <v>0.99093826854708311</v>
       </c>
       <c r="D9">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>1195.5023689534489</v>
       </c>
       <c r="L9">
@@ -2310,8 +2412,11 @@
       <c r="M9">
         <v>0.88270000000000004</v>
       </c>
-    </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N9">
+        <v>0.98</v>
+      </c>
+    </row>
+    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>8.8368208117631699</v>
       </c>
@@ -2319,15 +2424,15 @@
         <v>2.84391177622134E-2</v>
       </c>
       <c r="C10">
-        <f t="shared" si="0"/>
-        <v>0.98210324392035508</v>
+        <f t="shared" si="1"/>
+        <v>0.99101122290333077</v>
       </c>
       <c r="D10">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>1131.6286946419077</v>
       </c>
     </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>9.3708182885978992</v>
       </c>
@@ -2335,15 +2440,15 @@
         <v>2.8628355157262801E-2</v>
       </c>
       <c r="C11">
-        <f t="shared" si="0"/>
-        <v>0.98198523584194775</v>
+        <f t="shared" si="1"/>
+        <v>0.99095168189067007</v>
       </c>
       <c r="D11">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>1067.142664815907</v>
       </c>
     </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>9.8256840823073901</v>
       </c>
@@ -2351,15 +2456,15 @@
         <v>3.3693826945664897E-2</v>
       </c>
       <c r="C12">
-        <f t="shared" si="0"/>
-        <v>0.97883168162901868</v>
+        <f t="shared" si="1"/>
+        <v>0.98935922779798169</v>
       </c>
       <c r="D12">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>1017.7408429003424</v>
       </c>
     </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>10.320441988950201</v>
       </c>
@@ -2367,15 +2472,15 @@
         <v>3.68508287292817E-2</v>
       </c>
       <c r="C13">
-        <f t="shared" si="0"/>
-        <v>0.97687138709633181</v>
+        <f t="shared" si="1"/>
+        <v>0.98836804232853048</v>
       </c>
       <c r="D13">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>968.95074946467514</v>
       </c>
     </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>10.81389481011</v>
       </c>
@@ -2383,15 +2488,15 @@
         <v>3.7889241745334298E-2</v>
       </c>
       <c r="C14">
-        <f t="shared" si="0"/>
-        <v>0.97622745798386135</v>
+        <f t="shared" si="1"/>
+        <v>0.98804223491906529</v>
       </c>
       <c r="D14">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>924.73620056401114</v>
       </c>
     </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>11.287336320528899</v>
       </c>
@@ -2399,15 +2504,15 @@
         <v>3.9775960325401302E-2</v>
       </c>
       <c r="C15">
-        <f t="shared" si="0"/>
-        <v>0.9750585731075373</v>
+        <f t="shared" si="1"/>
+        <v>0.9874505421070654</v>
       </c>
       <c r="D15">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>885.94861675313507</v>
       </c>
     </row>
-    <row r="16" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>11.7814416844303</v>
       </c>
@@ -2415,11 +2520,11 @@
         <v>4.1873667725236E-2</v>
       </c>
       <c r="C16">
-        <f t="shared" si="0"/>
-        <v>0.97376061665124869</v>
+        <f t="shared" si="1"/>
+        <v>0.98679309718463715</v>
       </c>
       <c r="D16">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>848.79255594121776</v>
       </c>
     </row>
@@ -2431,11 +2536,11 @@
         <v>4.4607821812328703E-2</v>
       </c>
       <c r="C17">
-        <f t="shared" si="0"/>
-        <v>0.97207145208219081</v>
+        <f t="shared" si="1"/>
+        <v>0.98593683980374258</v>
       </c>
       <c r="D17">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>815.96649095717316</v>
       </c>
     </row>
@@ -2447,11 +2552,11 @@
         <v>4.4798799321355498E-2</v>
       </c>
       <c r="C18">
-        <f t="shared" si="0"/>
-        <v>0.97195357542666172</v>
+        <f t="shared" si="1"/>
+        <v>0.98587705898182953</v>
       </c>
       <c r="D18">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>784.41609849648478</v>
       </c>
     </row>
@@ -2463,11 +2568,11 @@
         <v>4.9014225431765701E-2</v>
       </c>
       <c r="C19">
-        <f t="shared" si="0"/>
-        <v>0.96935533342465818</v>
+        <f t="shared" si="1"/>
+        <v>0.98455844591606556</v>
       </c>
       <c r="D19">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>753.90448203709127</v>
       </c>
     </row>
@@ -2479,11 +2584,11 @@
         <v>5.1961108452603599E-2</v>
       </c>
       <c r="C20">
-        <f t="shared" si="0"/>
-        <v>0.96754310328906923</v>
+        <f t="shared" si="1"/>
+        <v>0.98363768903446824</v>
       </c>
       <c r="D20">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>728.97771237933705</v>
       </c>
     </row>
@@ -2495,11 +2600,11 @@
         <v>5.3846956975681898E-2</v>
       </c>
       <c r="C21">
-        <f t="shared" si="0"/>
-        <v>0.96638515052961627</v>
+        <f t="shared" si="1"/>
+        <v>0.98304890546178636</v>
       </c>
       <c r="D21">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>703.63987547714316</v>
       </c>
     </row>
@@ -2511,11 +2616,11 @@
         <v>5.7853134380301902E-2</v>
       </c>
       <c r="C22">
-        <f t="shared" si="0"/>
-        <v>0.96392986580602735</v>
+        <f t="shared" si="1"/>
+        <v>0.98179930016578609</v>
       </c>
       <c r="D22">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>681.84784414228568</v>
       </c>
     </row>
@@ -2527,11 +2632,11 @@
         <v>5.8465219471875399E-2</v>
       </c>
       <c r="C23">
-        <f t="shared" si="0"/>
-        <v>0.96355528409721891</v>
+        <f t="shared" si="1"/>
+        <v>0.98160851875746213</v>
       </c>
       <c r="D23">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>656.99480680574584</v>
       </c>
     </row>
@@ -2543,11 +2648,11 @@
         <v>5.99308304693957E-2</v>
       </c>
       <c r="C24">
-        <f t="shared" si="0"/>
-        <v>0.96265895601620377</v>
+        <f t="shared" si="1"/>
+        <v>0.98115185166018193</v>
       </c>
       <c r="D24">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>639.69700174207333</v>
       </c>
     </row>
@@ -2559,11 +2664,11 @@
         <v>6.0331926741201497E-2</v>
       </c>
       <c r="C25">
-        <f t="shared" si="0"/>
-        <v>0.9624138017243471</v>
+        <f t="shared" si="1"/>
+        <v>0.98102691182472013</v>
       </c>
       <c r="D25">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>618.56197190678847</v>
       </c>
     </row>
@@ -2575,11 +2680,11 @@
         <v>6.2217775264279802E-2</v>
       </c>
       <c r="C26">
-        <f t="shared" si="0"/>
-        <v>0.96126198769802218</v>
+        <f t="shared" si="1"/>
+        <v>0.9804396910050216</v>
       </c>
       <c r="D26">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>600.22194660226137</v>
       </c>
     </row>
@@ -2591,11 +2696,11 @@
         <v>6.5587505981641703E-2</v>
       </c>
       <c r="C27">
-        <f t="shared" si="0"/>
-        <v>0.95920729855226128</v>
+        <f t="shared" si="1"/>
+        <v>0.97939128980824686</v>
       </c>
       <c r="D27">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>583.60562507775501</v>
       </c>
     </row>
@@ -2607,11 +2712,11 @@
         <v>8.5323453356222601E-2</v>
       </c>
       <c r="C28">
-        <f t="shared" si="0"/>
-        <v>0.94726121190891122</v>
+        <f t="shared" si="1"/>
+        <v>0.97327345176415414</v>
       </c>
       <c r="D28">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>532.50096909876811</v>
       </c>
     </row>
@@ -2623,11 +2728,11 @@
         <v>9.6731784697625195E-2</v>
       </c>
       <c r="C29">
-        <f t="shared" si="0"/>
-        <v>0.94042377270332422</v>
+        <f t="shared" si="1"/>
+        <v>0.96975449094259125</v>
       </c>
       <c r="D29">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>493.57279606162859</v>
       </c>
     </row>
@@ -2639,11 +2744,11 @@
         <v>0.107596862165627</v>
       </c>
       <c r="C30">
-        <f t="shared" si="0"/>
-        <v>0.93395781523444621</v>
+        <f t="shared" si="1"/>
+        <v>0.96641492912436233</v>
       </c>
       <c r="D30">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>446.72135125952605</v>
       </c>
     </row>
@@ -2655,11 +2760,11 @@
         <v>0.13090245333449099</v>
       </c>
       <c r="C31">
-        <f t="shared" si="0"/>
-        <v>0.92023789773894971</v>
+        <f t="shared" si="1"/>
+        <v>0.95929030941574189</v>
       </c>
       <c r="D31">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>403.74361460158957</v>
       </c>
     </row>
@@ -2671,11 +2776,11 @@
         <v>0.16686585975358001</v>
       </c>
       <c r="C32">
-        <f t="shared" si="0"/>
-        <v>0.89946078683566144</v>
+        <f t="shared" si="1"/>
+        <v>0.94839906518071881</v>
       </c>
       <c r="D32">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>368.30300423173588</v>
       </c>
     </row>
@@ -2687,11 +2792,11 @@
         <v>0.174693244443341</v>
       </c>
       <c r="C33">
-        <f t="shared" si="0"/>
-        <v>0.89500120868557154</v>
+        <f t="shared" si="1"/>
+        <v>0.94604503523118366</v>
       </c>
       <c r="D33">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>356.31984737718471</v>
       </c>
     </row>
@@ -2703,11 +2808,11 @@
         <v>0.186540190206229</v>
       </c>
       <c r="C34">
-        <f t="shared" si="0"/>
-        <v>0.88829354601364108</v>
+        <f t="shared" si="1"/>
+        <v>0.94249326046059401</v>
       </c>
       <c r="D34">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>345.72394558959456</v>
       </c>
     </row>
@@ -2719,11 +2824,11 @@
         <v>0.19303222855149499</v>
       </c>
       <c r="C35">
-        <f t="shared" si="0"/>
-        <v>0.8846391430163093</v>
+        <f t="shared" si="1"/>
+        <v>0.94055257323358021</v>
       </c>
       <c r="D35">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>335.74235855513052</v>
       </c>
     </row>
@@ -2735,11 +2840,11 @@
         <v>0.20464635225274799</v>
       </c>
       <c r="C36">
-        <f t="shared" si="0"/>
-        <v>0.87813895595792524</v>
+        <f t="shared" si="1"/>
+        <v>0.93709068715782529</v>
       </c>
       <c r="D36">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>326.31885888673145</v>
       </c>
     </row>
@@ -2751,11 +2856,11 @@
         <v>0.21509636564582099</v>
       </c>
       <c r="C37">
-        <f t="shared" si="0"/>
-        <v>0.87233112889308773</v>
+        <f t="shared" si="1"/>
+        <v>0.93398668560803788</v>
       </c>
       <c r="D37">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>317.41036108359947</v>
       </c>
     </row>
@@ -2767,11 +2872,11 @@
         <v>0.22554637903889399</v>
       </c>
       <c r="C38">
-        <f t="shared" si="0"/>
-        <v>0.86656171357958656</v>
+        <f t="shared" si="1"/>
+        <v>0.9308929656945456</v>
       </c>
       <c r="D38">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>308.97534094584682</v>
       </c>
     </row>
@@ -2783,11 +2888,11 @@
         <v>0.23879025717159599</v>
       </c>
       <c r="C39">
-        <f t="shared" si="0"/>
-        <v>0.85930460702813538</v>
+        <f t="shared" si="1"/>
+        <v>0.9269868429638769</v>
       </c>
       <c r="D39">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>300.97605074037284</v>
       </c>
     </row>
@@ -2799,11 +2904,11 @@
         <v>0.248541804379763</v>
       </c>
       <c r="C40">
-        <f t="shared" si="0"/>
-        <v>0.85400003365820532</v>
+        <f t="shared" si="1"/>
+        <v>0.9241212223827594</v>
       </c>
       <c r="D40">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>293.38166777767316</v>
       </c>
     </row>
@@ -2815,11 +2920,11 @@
         <v>0.25410255447848601</v>
       </c>
       <c r="C41">
-        <f t="shared" si="0"/>
-        <v>0.85098981215698355</v>
+        <f t="shared" si="1"/>
+        <v>0.92249109055696765</v>
       </c>
       <c r="D41">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>286.16242879439375</v>
       </c>
     </row>
@@ -2831,11 +2936,11 @@
         <v>0.258964838392302</v>
       </c>
       <c r="C42">
-        <f t="shared" si="0"/>
-        <v>0.84836639037710848</v>
+        <f t="shared" si="1"/>
+        <v>0.92106807043622374</v>
       </c>
       <c r="D42">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>279.29015511039432</v>
       </c>
     </row>
@@ -2847,11 +2952,11 @@
         <v>0.28827343877786799</v>
       </c>
       <c r="C43">
-        <f t="shared" si="0"/>
-        <v>0.83272349256072653</v>
+        <f t="shared" si="1"/>
+        <v>0.91253684449490946</v>
       </c>
       <c r="D43">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>272.73319562582816</v>
       </c>
     </row>
@@ -2863,11 +2968,11 @@
         <v>0.31758203916343403</v>
       </c>
       <c r="C44">
-        <f t="shared" si="0"/>
-        <v>0.81736903173910214</v>
+        <f t="shared" si="1"/>
+        <v>0.90408463748650336</v>
       </c>
       <c r="D44">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>266.47705231527289</v>
       </c>
     </row>
@@ -2879,11 +2984,11 @@
         <v>0.34968450428862502</v>
       </c>
       <c r="C45">
-        <f t="shared" si="0"/>
-        <v>0.80087559168640787</v>
+        <f t="shared" si="1"/>
+        <v>0.8949165277758635</v>
       </c>
       <c r="D45">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>260.50075605636232</v>
       </c>
     </row>
@@ -2895,24 +3000,24 @@
         <v>0.37017684265783202</v>
       </c>
       <c r="C46">
-        <f t="shared" si="0"/>
-        <v>0.79052160248225001</v>
+        <f t="shared" si="1"/>
+        <v>0.88911281763466332</v>
       </c>
       <c r="D46">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>256.83524758947482</v>
       </c>
     </row>
     <row r="47" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A47">
         <f>10000/D47</f>
-        <v>52.631578947368418</v>
+        <v>50</v>
       </c>
       <c r="C47">
-        <v>0.71</v>
+        <v>0.87</v>
       </c>
       <c r="D47">
-        <v>190</v>
+        <v>200</v>
       </c>
       <c r="E47" t="s">
         <v>10</v>
@@ -2924,7 +3029,7 @@
         <v>55.555555555555557</v>
       </c>
       <c r="C48">
-        <v>0.6</v>
+        <v>0.86</v>
       </c>
       <c r="D48">
         <v>180</v>

</xml_diff>